<commit_message>
pad nicknames for better ordering
</commit_message>
<xml_diff>
--- a/address_concept_map.xlsx
+++ b/address_concept_map.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R25"/>
+  <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -457,7 +457,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>home_address_1</t>
+          <t>home_address_01</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -549,7 +549,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>home_address_2</t>
+          <t>home_address_02</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -641,7 +641,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>home_address_3</t>
+          <t>home_address_03</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -733,7 +733,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>home_address_4</t>
+          <t>home_address_04</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -825,7 +825,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>home_address_5</t>
+          <t>home_address_05</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -917,7 +917,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>home_address_6</t>
+          <t>home_address_06</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1009,7 +1009,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>home_address_7</t>
+          <t>home_address_07</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>home_address_8</t>
+          <t>home_address_08</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1193,7 +1193,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>home_address_9</t>
+          <t>home_address_09</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1469,7 +1469,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>seasonal_address_1</t>
+          <t>seasonal_address_01</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1561,7 +1561,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>seasonal_address_2</t>
+          <t>seasonal_address_02</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1653,7 +1653,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>seasonal_address_3</t>
+          <t>seasonal_address_03</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1745,7 +1745,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>seasonal_address_4</t>
+          <t>seasonal_address_04</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1837,7 +1837,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>seasonal_address_5</t>
+          <t>seasonal_address_05</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1929,7 +1929,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>seasonal_address_6</t>
+          <t>seasonal_address_06</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -2021,7 +2021,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>seasonal_address_7</t>
+          <t>seasonal_address_07</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -2113,7 +2113,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>seasonal_address_8</t>
+          <t>seasonal_address_08</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -2205,7 +2205,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>seasonal_address_9</t>
+          <t>seasonal_address_09</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -2384,274 +2384,366 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>596318751</t>
+          <t>632533534</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>current_work_address_1</t>
+          <t>childhood_address_01</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>493984171</t>
+          <t>284547539</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>253017624</t>
+          <t>802585033</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>404141282</t>
+          <t>746533238</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>959804472</t>
+          <t>128827522</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>774707280</t>
+          <t>439447560</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>182144476</t>
+          <t>286781627</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>294634899</t>
+          <t>733929451</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>263588196</t>
+          <t>264797252</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>583500714</t>
+          <t>890792569</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>742105146</t>
+          <t>451394598</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>101341673</t>
+          <t>984908796</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>237204853</t>
+          <t>847327251</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>845811202</t>
+          <t>469914719</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>510435329</t>
+          <t>952124199</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>520264332</t>
+          <t>204186397</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>Current Work</t>
+          <t>Childhood</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>992180692</t>
+          <t>596318751</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>previous_work_address_1</t>
+          <t>current_work_address_01</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>903896611</t>
+          <t>493984171</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>855583262</t>
+          <t>253017624</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>371588177</t>
+          <t>404141282</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>962868433</t>
+          <t>959804472</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>108530997</t>
+          <t>774707280</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>110852652</t>
+          <t>182144476</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>867109611</t>
+          <t>294634899</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>350394531</t>
+          <t>263588196</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>652022112</t>
+          <t>583500714</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>730666903</t>
+          <t>742105146</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>168091937</t>
+          <t>101341673</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>132779701</t>
+          <t>237204853</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>733317111</t>
+          <t>845811202</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>584350267</t>
+          <t>510435329</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>840147245</t>
+          <t>520264332</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>Previous Work</t>
+          <t>Current Work</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>992180692</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>previous_work_address_01</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>903896611</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>855583262</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>371588177</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>962868433</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>108530997</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>110852652</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>867109611</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>350394531</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>652022112</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>730666903</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>168091937</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>132779701</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>733317111</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>584350267</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>840147245</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>Previous Work</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
           <t>914696832</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>school_address_1</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>school_address_01</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
         <is>
           <t>970996351</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>249657148</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>190883115</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>161170041</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="G26" t="inlineStr">
         <is>
           <t>660217075</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr">
+      <c r="H26" t="inlineStr">
         <is>
           <t>884494489</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr">
+      <c r="I26" t="inlineStr">
         <is>
           <t>403679963</t>
         </is>
       </c>
-      <c r="J25" t="inlineStr">
+      <c r="J26" t="inlineStr">
         <is>
           <t>668887646</t>
         </is>
       </c>
-      <c r="K25" t="inlineStr">
+      <c r="K26" t="inlineStr">
         <is>
           <t>225725599</t>
         </is>
       </c>
-      <c r="L25" t="inlineStr">
+      <c r="L26" t="inlineStr">
         <is>
           <t>977086216</t>
         </is>
       </c>
-      <c r="M25" t="inlineStr">
+      <c r="M26" t="inlineStr">
         <is>
           <t>997041632</t>
         </is>
       </c>
-      <c r="N25" t="inlineStr">
+      <c r="N26" t="inlineStr">
         <is>
           <t>147113671</t>
         </is>
       </c>
-      <c r="O25" t="inlineStr">
+      <c r="O26" t="inlineStr">
         <is>
           <t>443679537</t>
         </is>
       </c>
-      <c r="P25" t="inlineStr">
+      <c r="P26" t="inlineStr">
         <is>
           <t>494271326</t>
         </is>
       </c>
-      <c r="Q25" t="inlineStr">
+      <c r="Q26" t="inlineStr">
         <is>
           <t>952170182</t>
         </is>
       </c>
-      <c r="R25" t="inlineStr">
+      <c r="R26" t="inlineStr">
         <is>
           <t>School</t>
         </is>

</xml_diff>